<commit_message>
VAHAN table update - test 2
</commit_message>
<xml_diff>
--- a/high_value_datasets.xlsx
+++ b/high_value_datasets.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\thinkpad\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{718DA0BC-F0AB-4E66-87F6-474FDD5E5B31}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{87553C34-7200-45DC-B50D-DDE14BFD24A0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{4EB7C4AF-9817-468B-9337-4C375DB1459C}"/>
   </bookViews>
@@ -1061,7 +1061,7 @@
   <dimension ref="A1:E85"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A74" workbookViewId="0">
-      <selection activeCell="A85" sqref="A85"/>
+      <selection activeCell="B85" sqref="B85"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2354,11 +2354,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_activity xmlns="2ae390d3-5390-45a7-b10d-acc3dc2cfb8d" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2595,20 +2596,17 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_activity xmlns="2ae390d3-5390-45a7-b10d-acc3dc2cfb8d" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F9106F8C-F34C-4D94-BE95-9AEFF7EE5E76}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7CC16AD0-BEA8-4D4A-967D-54E7DFE02C23}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="2ae390d3-5390-45a7-b10d-acc3dc2cfb8d"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -2633,9 +2631,11 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7CC16AD0-BEA8-4D4A-967D-54E7DFE02C23}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F9106F8C-F34C-4D94-BE95-9AEFF7EE5E76}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="2ae390d3-5390-45a7-b10d-acc3dc2cfb8d"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>